<commit_message>
Added Architectural Diagram using Star UML
This will help us to define the generic component and discuss on the
development. Added the same component view of server in excel sheet.
</commit_message>
<xml_diff>
--- a/ProjectRequirements/ProjectPlanning.xlsx
+++ b/ProjectRequirements/ProjectPlanning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Deployment Diagram" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="Tools Required" sheetId="4" r:id="rId4"/>
     <sheet name="TestPlan" sheetId="5" r:id="rId5"/>
     <sheet name="Backend Database Requirement" sheetId="6" r:id="rId6"/>
+    <sheet name="Server Component View" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -586,6 +587,51 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7839075" cy="3838575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -887,7 +933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:Z111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2498,4 +2544,17 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>